<commit_message>
updating Individual Assessment SET08103 Group B.xlsx
</commit_message>
<xml_diff>
--- a/documentation/Individual Assessment SET08103 Group B.xlsx
+++ b/documentation/Individual Assessment SET08103 Group B.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livenapierac-my.sharepoint.com/personal/40343450_live_napier_ac_uk/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott McMahon\IdeaProjects\SEMCourseworkGroupB\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{5B7F80C4-48D9-4290-A981-FA24C1CA6E2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D5A6E601-85F3-4A79-99B1-028D0E70254D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A0678D-D088-41D5-BDB5-1A240F507CD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19440" yWindow="240" windowWidth="37920" windowHeight="20520" xr2:uid="{FE433FBF-82ED-4F1C-B405-C0C664F2394C}"/>
   </bookViews>
   <sheets>
     <sheet name="Individual Assessment SET08103 " sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -87,7 +87,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -452,17 +452,17 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,7 +482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>40343450</v>
       </c>
@@ -494,43 +494,49 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>40456918</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <v>25</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>40456785</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>25</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>40456784</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>25</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3">
         <f>SUM(B2:B5)</f>
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ref="C6:F6" si="0">SUM(C2:C5)</f>
@@ -549,7 +555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="75">
+    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -565,6 +571,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100094F3ECC3101F94CA5378CA3B6BDFBC8" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b01c64cf6e197e395573538ffc1645a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="292d26df-bb38-4049-b6a8-318c56da4d22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b250f74f05ba24f16c04c2c927008d2b" ns3:_="">
     <xsd:import namespace="292d26df-bb38-4049-b6a8-318c56da4d22"/>
@@ -710,29 +731,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6510804E-2BA4-4D96-8250-A09FE28718E4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B73E0ABA-79A7-4D0C-B05B-CAC96BC3BEE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89B75AC2-1111-4C94-9F9E-BB4EBD374D51}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89B75AC2-1111-4C94-9F9E-BB4EBD374D51}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B73E0ABA-79A7-4D0C-B05B-CAC96BC3BEE8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6510804E-2BA4-4D96-8250-A09FE28718E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="292d26df-bb38-4049-b6a8-318c56da4d22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>